<commit_message>
Improved refrence object length calculation and solved the problem due to different orientation as in test21/23.png
</commit_message>
<xml_diff>
--- a/Image Processing Result.xlsx
+++ b/Image Processing Result.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="15">
   <si>
     <t>Activity</t>
   </si>
@@ -56,10 +56,22 @@
     <t>Pipe</t>
   </si>
   <si>
-    <t>4cm away</t>
-  </si>
-  <si>
-    <t>3.5cm away</t>
+    <t xml:space="preserve">Out of range </t>
+  </si>
+  <si>
+    <t>Same as 0 and 1</t>
+  </si>
+  <si>
+    <t>The wrapping caused the image to go outiside the frame and so processing could not be applied</t>
+  </si>
+  <si>
+    <t>Had to change things like new_X and new_Y and also the way self.X_Cordinate</t>
+  </si>
+  <si>
+    <t>1 cm Away</t>
+  </si>
+  <si>
+    <t>Fixed the error</t>
   </si>
 </sst>
 </file>
@@ -104,16 +116,20 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -392,264 +408,328 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" customWidth="1"/>
-    <col min="2" max="2" width="20.1640625" customWidth="1"/>
-    <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="44.5" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="20.1640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="21" style="3" customWidth="1"/>
+    <col min="4" max="4" width="44.5" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="2">
+      <c r="B4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="2">
+      <c r="B5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="2">
+      <c r="B6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="2">
+      <c r="B7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8">
+      <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="2">
+      <c r="B8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="2">
+      <c r="B9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10">
+      <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="2">
+      <c r="B10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11">
+      <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="2">
+      <c r="B11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A12">
+      <c r="A12" s="3">
         <v>11</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C12" s="5">
         <v>0.33</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A13">
+      <c r="A13" s="3">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="4">
         <v>1.1599999999999999</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14">
+      <c r="A14" s="3">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="2">
+      <c r="B14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15">
+      <c r="A15" s="3">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="2">
+      <c r="B15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16">
+      <c r="A16" s="3">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17">
+      <c r="B16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
-        <v>2</v>
-      </c>
-      <c r="C17" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="B17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>0</v>
-      </c>
-      <c r="B19" t="s">
+    <row r="19" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A19" s="3">
+        <v>0</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20">
+      <c r="C19" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="3">
         <v>1</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21">
+      <c r="C20" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="3">
         <v>18</v>
       </c>
-      <c r="B21" t="s">
-        <v>2</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="B21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="3">
+        <v>19</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="3">
+        <v>17</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="3">
+        <v>20</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A25" s="3">
+        <v>21</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" s="4">
+        <v>0</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="3">
+        <v>23</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="3">
+        <v>22</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>19</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="D27" s="3" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>17</v>
-      </c>
-      <c r="B23" t="s">
-        <v>2</v>
-      </c>
-      <c r="C23" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>